<commit_message>
added some datasheets and started wiring stuff up.
</commit_message>
<xml_diff>
--- a/electronics/mbed-motherboard/pin-allocation.xlsx
+++ b/electronics/mbed-motherboard/pin-allocation.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="56">
   <si>
     <t>Pin Name</t>
   </si>
@@ -174,9 +174,6 @@
     <t>spindle on/off</t>
   </si>
   <si>
-    <t>analog pins</t>
-  </si>
-  <si>
     <t>pwm out mosfet</t>
   </si>
   <si>
@@ -184,6 +181,12 @@
   </si>
   <si>
     <t>tool zeroing</t>
+  </si>
+  <si>
+    <t>debug</t>
+  </si>
+  <si>
+    <t>debug port</t>
   </si>
 </sst>
 </file>
@@ -255,8 +258,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -284,7 +289,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="21">
+  <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -295,6 +300,7 @@
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -305,6 +311,7 @@
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -637,7 +644,7 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -702,7 +709,7 @@
       <c r="G3">
         <v>4</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="2">
         <f>F3*G3</f>
         <v>12</v>
       </c>
@@ -727,7 +734,7 @@
         <f>G3</f>
         <v>4</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="2">
         <f>F4*G4</f>
         <v>4</v>
       </c>
@@ -740,7 +747,7 @@
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -748,7 +755,7 @@
       <c r="G5">
         <v>1</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="2">
         <f>F5*G5</f>
         <v>1</v>
       </c>
@@ -761,7 +768,7 @@
         <v>19</v>
       </c>
       <c r="E6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -769,7 +776,7 @@
       <c r="G6">
         <v>1</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="2">
         <f>F6*G6</f>
         <v>1</v>
       </c>
@@ -791,6 +798,7 @@
         <v>1</v>
       </c>
       <c r="H7" s="2">
+        <f>F7*G7</f>
         <v>4</v>
       </c>
     </row>
@@ -811,6 +819,7 @@
         <v>1</v>
       </c>
       <c r="H8" s="2">
+        <f>F8*G8</f>
         <v>1</v>
       </c>
     </row>
@@ -822,15 +831,16 @@
         <v>7</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="F9" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G9" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H9" s="2">
+        <f>F9*G9</f>
         <v>2</v>
       </c>
     </row>
@@ -841,17 +851,21 @@
       <c r="B10" t="s">
         <v>17</v>
       </c>
+      <c r="C10" t="s">
+        <v>54</v>
+      </c>
       <c r="E10" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F10" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H10" s="2">
-        <v>1</v>
+        <f>F10*G10</f>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -860,6 +874,9 @@
       </c>
       <c r="B11" t="s">
         <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>54</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -868,7 +885,7 @@
       </c>
       <c r="H11" s="3">
         <f>SUM(H3:H10)</f>
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -901,7 +918,7 @@
       </c>
       <c r="H13" s="3">
         <f>H12-H11</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:8">

</xml_diff>

<commit_message>
added ttl cable and started assigning more pins.
</commit_message>
<xml_diff>
--- a/electronics/mbed-motherboard/pin-allocation.xlsx
+++ b/electronics/mbed-motherboard/pin-allocation.xlsx
@@ -174,9 +174,6 @@
     <t>spindle on/off</t>
   </si>
   <si>
-    <t>pwm out mosfet</t>
-  </si>
-  <si>
     <t>door switch</t>
   </si>
   <si>
@@ -187,6 +184,9 @@
   </si>
   <si>
     <t>debug port</t>
+  </si>
+  <si>
+    <t>buzzer / pwm / io?</t>
   </si>
 </sst>
 </file>
@@ -644,7 +644,7 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -710,7 +710,7 @@
         <v>4</v>
       </c>
       <c r="H3" s="2">
-        <f>F3*G3</f>
+        <f t="shared" ref="H3:H10" si="0">F3*G3</f>
         <v>12</v>
       </c>
     </row>
@@ -735,7 +735,7 @@
         <v>4</v>
       </c>
       <c r="H4" s="2">
-        <f>F4*G4</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
@@ -747,7 +747,7 @@
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -756,7 +756,7 @@
         <v>1</v>
       </c>
       <c r="H5" s="2">
-        <f>F5*G5</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -768,7 +768,7 @@
         <v>19</v>
       </c>
       <c r="E6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -777,7 +777,7 @@
         <v>1</v>
       </c>
       <c r="H6" s="2">
-        <f>F6*G6</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -798,7 +798,7 @@
         <v>1</v>
       </c>
       <c r="H7" s="2">
-        <f>F7*G7</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
@@ -819,7 +819,7 @@
         <v>1</v>
       </c>
       <c r="H8" s="2">
-        <f>F8*G8</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -831,7 +831,7 @@
         <v>7</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F9" s="2">
         <v>2</v>
@@ -840,7 +840,7 @@
         <v>1</v>
       </c>
       <c r="H9" s="2">
-        <f>F9*G9</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -852,20 +852,20 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="F10" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" s="2">
-        <f>F10*G10</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -876,7 +876,7 @@
         <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -885,7 +885,7 @@
       </c>
       <c r="H11" s="3">
         <f>SUM(H3:H10)</f>
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -918,7 +918,7 @@
       </c>
       <c r="H13" s="3">
         <f>H12-H11</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:8">

</xml_diff>

<commit_message>
switched to the lpcxpresso based on arthurs suggestion.
</commit_message>
<xml_diff>
--- a/electronics/mbed-motherboard/pin-allocation.xlsx
+++ b/electronics/mbed-motherboard/pin-allocation.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="61">
   <si>
     <t>Pin Name</t>
   </si>
@@ -153,15 +153,9 @@
     <t>instances</t>
   </si>
   <si>
-    <t>stepper</t>
-  </si>
-  <si>
     <t>total</t>
   </si>
   <si>
-    <t>endstops</t>
-  </si>
-  <si>
     <t>sd card</t>
   </si>
   <si>
@@ -186,7 +180,28 @@
     <t>debug port</t>
   </si>
   <si>
-    <t>buzzer / pwm / io?</t>
+    <t>buzzer</t>
+  </si>
+  <si>
+    <t>pwm mosfets</t>
+  </si>
+  <si>
+    <t>analog inputs</t>
+  </si>
+  <si>
+    <t>current monitoring</t>
+  </si>
+  <si>
+    <t>spindle rpm</t>
+  </si>
+  <si>
+    <t>axes encoders</t>
+  </si>
+  <si>
+    <t>axes endstops</t>
+  </si>
+  <si>
+    <t>axes steppers</t>
   </si>
 </sst>
 </file>
@@ -258,8 +273,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -289,7 +320,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="39">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -301,6 +332,14 @@
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -312,6 +351,14 @@
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -644,7 +691,7 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -687,7 +734,7 @@
         <v>43</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -701,17 +748,17 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="F3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H3" s="2">
-        <f t="shared" ref="H3:H10" si="0">F3*G3</f>
-        <v>12</v>
+        <f t="shared" ref="H3:H4" si="0">F3*G3</f>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -725,18 +772,18 @@
         <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4">
         <f>G3</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H4" s="2">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -746,18 +793,19 @@
       <c r="C5" t="s">
         <v>5</v>
       </c>
-      <c r="E5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
+      <c r="E5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F5" s="2">
+        <v>2</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <f>G3</f>
+        <v>5</v>
       </c>
       <c r="H5" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>F5*G5</f>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -768,7 +816,7 @@
         <v>19</v>
       </c>
       <c r="E6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -777,7 +825,7 @@
         <v>1</v>
       </c>
       <c r="H6" s="2">
-        <f t="shared" si="0"/>
+        <f>F6*G6</f>
         <v>1</v>
       </c>
     </row>
@@ -788,18 +836,18 @@
       <c r="B7" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="F7" s="2">
-        <v>4</v>
-      </c>
-      <c r="G7" s="2">
+      <c r="E7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
         <v>1</v>
       </c>
       <c r="H7" s="2">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f>F7*G7</f>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -810,17 +858,17 @@
         <v>4</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F8" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G8" s="2">
         <v>1</v>
       </c>
       <c r="H8" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>F8*G8</f>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -831,17 +879,17 @@
         <v>7</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="F9" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G9" s="2">
         <v>1</v>
       </c>
       <c r="H9" s="2">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>F9*G9</f>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -852,19 +900,19 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>53</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="F10" s="2">
-        <v>1</v>
-      </c>
-      <c r="G10" s="2">
+        <v>51</v>
+      </c>
+      <c r="E10" t="s">
+        <v>57</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
         <v>1</v>
       </c>
       <c r="H10" s="2">
-        <f t="shared" si="0"/>
+        <f>F10*G10</f>
         <v>1</v>
       </c>
     </row>
@@ -876,16 +924,20 @@
         <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>53</v>
-      </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="H11" s="3">
-        <f>SUM(H3:H10)</f>
-        <v>26</v>
+        <v>51</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11" s="2">
+        <v>2</v>
+      </c>
+      <c r="G11" s="2">
+        <v>1</v>
+      </c>
+      <c r="H11" s="2">
+        <f>F11*G11</f>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -895,13 +947,18 @@
       <c r="B12" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="H12" s="3">
-        <v>26</v>
+      <c r="E12" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1</v>
+      </c>
+      <c r="G12" s="2">
+        <v>1</v>
+      </c>
+      <c r="H12" s="2">
+        <f>F12*G12</f>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -911,14 +968,18 @@
       <c r="B13" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H13" s="3">
-        <f>H12-H11</f>
-        <v>0</v>
+      <c r="E13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" s="2">
+        <v>1</v>
+      </c>
+      <c r="G13" s="2">
+        <v>3</v>
+      </c>
+      <c r="H13" s="2">
+        <f>F13*G13</f>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -928,6 +989,19 @@
       <c r="B14" t="s">
         <v>22</v>
       </c>
+      <c r="E14" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F14" s="2">
+        <v>1</v>
+      </c>
+      <c r="G14" s="2">
+        <v>3</v>
+      </c>
+      <c r="H14" s="2">
+        <f>F14*G14</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
@@ -936,6 +1010,19 @@
       <c r="B15" t="s">
         <v>22</v>
       </c>
+      <c r="E15" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F15" s="2">
+        <v>1</v>
+      </c>
+      <c r="G15" s="2">
+        <v>1</v>
+      </c>
+      <c r="H15" s="2">
+        <f>F15*G15</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
@@ -944,24 +1031,50 @@
       <c r="B16" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H16" s="3">
+        <f>SUM(H3:H15)</f>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>27</v>
       </c>
       <c r="B17" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H17" s="3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>28</v>
       </c>
       <c r="B18" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H18" s="3">
+        <f>H17-H16</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -969,7 +1082,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -977,7 +1090,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -985,7 +1098,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:8">
       <c r="A22" t="s">
         <v>33</v>
       </c>
@@ -993,7 +1106,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:8">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -1001,7 +1114,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:8">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -1009,7 +1122,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:8">
       <c r="A25" t="s">
         <v>36</v>
       </c>
@@ -1017,7 +1130,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:8">
       <c r="A26" t="s">
         <v>37</v>
       </c>
@@ -1025,7 +1138,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:8">
       <c r="A27" t="s">
         <v>38</v>
       </c>

</xml_diff>

<commit_message>
did a lot of work laying out and fleshing out the board with the new lpcxpresso
</commit_message>
<xml_diff>
--- a/electronics/mbed-motherboard/pin-allocation.xlsx
+++ b/electronics/mbed-motherboard/pin-allocation.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="62">
   <si>
     <t>Pin Name</t>
   </si>
@@ -202,6 +202,9 @@
   </si>
   <si>
     <t>axes steppers</t>
+  </si>
+  <si>
+    <t>step/dir/enable + protect</t>
   </si>
 </sst>
 </file>
@@ -688,10 +691,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -699,7 +702,7 @@
     <col min="5" max="5" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -714,7 +717,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -737,7 +740,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -760,8 +763,11 @@
         <f t="shared" ref="H3:H4" si="0">F3*G3</f>
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="J3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -786,7 +792,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -804,11 +810,11 @@
         <v>5</v>
       </c>
       <c r="H5" s="2">
-        <f>F5*G5</f>
+        <f t="shared" ref="H5:H15" si="1">F5*G5</f>
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -825,11 +831,11 @@
         <v>1</v>
       </c>
       <c r="H6" s="2">
-        <f>F6*G6</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -846,11 +852,11 @@
         <v>1</v>
       </c>
       <c r="H7" s="2">
-        <f>F7*G7</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -867,11 +873,11 @@
         <v>1</v>
       </c>
       <c r="H8" s="2">
-        <f>F8*G8</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -888,11 +894,11 @@
         <v>1</v>
       </c>
       <c r="H9" s="2">
-        <f>F9*G9</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -912,11 +918,11 @@
         <v>1</v>
       </c>
       <c r="H10" s="2">
-        <f>F10*G10</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -936,11 +942,11 @@
         <v>1</v>
       </c>
       <c r="H11" s="2">
-        <f>F11*G11</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -957,11 +963,11 @@
         <v>1</v>
       </c>
       <c r="H12" s="2">
-        <f>F12*G12</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -978,11 +984,11 @@
         <v>3</v>
       </c>
       <c r="H13" s="2">
-        <f>F13*G13</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -999,11 +1005,11 @@
         <v>3</v>
       </c>
       <c r="H14" s="2">
-        <f>F14*G14</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -1020,11 +1026,11 @@
         <v>1</v>
       </c>
       <c r="H15" s="2">
-        <f>F15*G15</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
did a bunch of work on the controller board.
</commit_message>
<xml_diff>
--- a/electronics/mbed-motherboard/pin-allocation.xlsx
+++ b/electronics/mbed-motherboard/pin-allocation.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="143">
   <si>
     <t>Pin Name</t>
   </si>
@@ -373,9 +373,6 @@
     <t>TOOLZERO</t>
   </si>
   <si>
-    <t>ANALOG</t>
-  </si>
-  <si>
     <t>MOSFET</t>
   </si>
   <si>
@@ -436,19 +433,22 @@
     <t>only protect left</t>
   </si>
   <si>
-    <t>how to control spindle?</t>
-  </si>
-  <si>
     <t>find buzzer footprint</t>
   </si>
   <si>
-    <t>find mosfets and add</t>
-  </si>
-  <si>
-    <t>add headers</t>
-  </si>
-  <si>
-    <t>look up circuit</t>
+    <t>CURRENT+</t>
+  </si>
+  <si>
+    <t>CURRENT-</t>
+  </si>
+  <si>
+    <t>ADC1</t>
+  </si>
+  <si>
+    <t>ADC2</t>
+  </si>
+  <si>
+    <t>status</t>
   </si>
 </sst>
 </file>
@@ -546,7 +546,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="77">
+  <cellStyleXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -624,19 +624,36 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="77">
+  <cellStyles count="85">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -675,6 +692,10 @@
     <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -713,6 +734,10 @@
     <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1045,7 +1070,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1064,14 +1089,17 @@
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="7" t="s">
         <v>15</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1088,8 +1116,8 @@
         <f t="shared" ref="D3:D4" si="0">B3*C3</f>
         <v>20</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>137</v>
+      <c r="E3" s="8" t="s">
+        <v>136</v>
       </c>
       <c r="F3" t="s">
         <v>31</v>
@@ -1110,8 +1138,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>125</v>
+      <c r="E4" s="4" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1129,8 +1157,8 @@
         <f t="shared" ref="D5:D15" si="1">B5*C5</f>
         <v>10</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>125</v>
+      <c r="E5" s="4" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1147,8 +1175,8 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>125</v>
+      <c r="E6" s="4" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1165,8 +1193,8 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>125</v>
+      <c r="E7" s="4" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1183,8 +1211,8 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="E8" s="5" t="s">
-        <v>125</v>
+      <c r="E8" s="4" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1201,8 +1229,8 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E9" s="6" t="s">
-        <v>138</v>
+      <c r="E9" s="4" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1219,8 +1247,8 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E10" s="5" t="s">
-        <v>125</v>
+      <c r="E10" s="4" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1237,8 +1265,8 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>125</v>
+      <c r="E11" s="4" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1255,8 +1283,8 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E12" s="6" t="s">
-        <v>139</v>
+      <c r="E12" s="5" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1273,8 +1301,8 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="E13" s="6" t="s">
-        <v>140</v>
+      <c r="E13" s="4" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1291,8 +1319,8 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="E14" s="6" t="s">
-        <v>141</v>
+      <c r="E14" s="4" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1309,8 +1337,8 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E15" s="6" t="s">
-        <v>142</v>
+      <c r="E15" s="4" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1360,28 +1388,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:11" ht="20">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="E1" s="4" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="E1" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="I1" s="4" t="s">
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="I1" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
@@ -1419,7 +1447,7 @@
       <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E3" t="s">
@@ -1428,17 +1456,17 @@
       <c r="F3" t="s">
         <v>60</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>120</v>
+      <c r="G3" s="4" t="s">
+        <v>119</v>
       </c>
       <c r="I3" t="s">
         <v>81</v>
       </c>
       <c r="J3" t="s">
+        <v>125</v>
+      </c>
+      <c r="K3" s="4" t="s">
         <v>126</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -1448,7 +1476,7 @@
       <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E4" t="s">
@@ -1457,13 +1485,13 @@
       <c r="F4" t="s">
         <v>62</v>
       </c>
-      <c r="G4" s="5" t="s">
-        <v>122</v>
+      <c r="G4" s="4" t="s">
+        <v>121</v>
       </c>
       <c r="I4" t="s">
         <v>82</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="K4" s="4" t="s">
         <v>115</v>
       </c>
     </row>
@@ -1474,7 +1502,7 @@
       <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E5" t="s">
@@ -1483,13 +1511,13 @@
       <c r="F5" t="s">
         <v>64</v>
       </c>
-      <c r="G5" s="5" t="s">
-        <v>124</v>
+      <c r="G5" s="4" t="s">
+        <v>123</v>
       </c>
       <c r="I5" t="s">
         <v>39</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="K5" s="4" t="s">
         <v>114</v>
       </c>
     </row>
@@ -1497,7 +1525,7 @@
       <c r="A6" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E6" t="s">
@@ -1506,13 +1534,13 @@
       <c r="F6" t="s">
         <v>66</v>
       </c>
-      <c r="G6" s="5" t="s">
-        <v>129</v>
+      <c r="G6" s="4" t="s">
+        <v>128</v>
       </c>
       <c r="I6" t="s">
         <v>83</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="K6" s="4" t="s">
         <v>116</v>
       </c>
     </row>
@@ -1523,8 +1551,8 @@
       <c r="B7" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>119</v>
+      <c r="C7" s="4" t="s">
+        <v>118</v>
       </c>
       <c r="E7" t="s">
         <v>67</v>
@@ -1532,8 +1560,8 @@
       <c r="F7" t="s">
         <v>68</v>
       </c>
-      <c r="G7" s="6" t="s">
-        <v>118</v>
+      <c r="G7" s="4" t="s">
+        <v>117</v>
       </c>
       <c r="I7" t="s">
         <v>84</v>
@@ -1546,8 +1574,8 @@
       <c r="B8" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>121</v>
+      <c r="C8" s="4" t="s">
+        <v>120</v>
       </c>
       <c r="E8" t="s">
         <v>69</v>
@@ -1555,8 +1583,8 @@
       <c r="F8" t="s">
         <v>68</v>
       </c>
-      <c r="G8" s="6" t="s">
-        <v>118</v>
+      <c r="G8" s="4" t="s">
+        <v>117</v>
       </c>
       <c r="I8" t="s">
         <v>86</v>
@@ -1569,8 +1597,8 @@
       <c r="B9" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>123</v>
+      <c r="C9" s="4" t="s">
+        <v>122</v>
       </c>
       <c r="E9" t="s">
         <v>70</v>
@@ -1578,8 +1606,8 @@
       <c r="F9" t="s">
         <v>68</v>
       </c>
-      <c r="G9" s="6" t="s">
-        <v>118</v>
+      <c r="G9" s="4" t="s">
+        <v>117</v>
       </c>
       <c r="I9" t="s">
         <v>87</v>
@@ -1592,8 +1620,8 @@
       <c r="B10" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>128</v>
+      <c r="C10" s="4" t="s">
+        <v>127</v>
       </c>
       <c r="E10" t="s">
         <v>71</v>
@@ -1601,14 +1629,14 @@
       <c r="F10" t="s">
         <v>68</v>
       </c>
-      <c r="G10" s="5" t="s">
-        <v>132</v>
+      <c r="G10" s="4" t="s">
+        <v>131</v>
       </c>
       <c r="I10" t="s">
         <v>85</v>
       </c>
-      <c r="J10" s="5" t="s">
-        <v>130</v>
+      <c r="K10" s="4" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1618,7 +1646,7 @@
       <c r="B11" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>22</v>
       </c>
       <c r="E11" t="s">
@@ -1627,8 +1655,8 @@
       <c r="F11" t="s">
         <v>68</v>
       </c>
-      <c r="G11" s="5" t="s">
-        <v>134</v>
+      <c r="G11" s="4" t="s">
+        <v>133</v>
       </c>
       <c r="I11" t="s">
         <v>88</v>
@@ -1641,7 +1669,7 @@
       <c r="B12" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>22</v>
       </c>
       <c r="E12" t="s">
@@ -1650,8 +1678,8 @@
       <c r="F12" t="s">
         <v>68</v>
       </c>
-      <c r="G12" s="5" t="s">
-        <v>133</v>
+      <c r="G12" s="4" t="s">
+        <v>132</v>
       </c>
       <c r="I12" t="s">
         <v>89</v>
@@ -1664,20 +1692,20 @@
       <c r="B13" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>117</v>
+      <c r="C13" s="4" t="s">
+        <v>138</v>
       </c>
       <c r="E13" t="s">
         <v>74</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="G13" s="4" t="s">
         <v>99</v>
       </c>
       <c r="I13" t="s">
         <v>90</v>
       </c>
-      <c r="J13" s="5" t="s">
-        <v>131</v>
+      <c r="K13" s="4" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1687,13 +1715,13 @@
       <c r="B14" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>117</v>
+      <c r="C14" s="4" t="s">
+        <v>139</v>
       </c>
       <c r="E14" t="s">
         <v>75</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="G14" s="4" t="s">
         <v>100</v>
       </c>
       <c r="I14" t="s">
@@ -1707,13 +1735,13 @@
       <c r="B15" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>117</v>
+      <c r="C15" s="4" t="s">
+        <v>140</v>
       </c>
       <c r="E15" t="s">
         <v>76</v>
       </c>
-      <c r="G15" s="5" t="s">
+      <c r="G15" s="4" t="s">
         <v>101</v>
       </c>
       <c r="I15" t="s">
@@ -1727,127 +1755,127 @@
       <c r="B16" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="6" t="s">
-        <v>117</v>
+      <c r="C16" s="4" t="s">
+        <v>141</v>
       </c>
       <c r="E16" t="s">
         <v>77</v>
       </c>
-      <c r="G16" s="5" t="s">
+      <c r="G16" s="4" t="s">
         <v>102</v>
       </c>
       <c r="I16" t="s">
         <v>93</v>
       </c>
-      <c r="J16" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10">
+      <c r="K16" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" t="s">
         <v>47</v>
       </c>
       <c r="B17" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="4" t="s">
         <v>109</v>
       </c>
       <c r="E17" t="s">
         <v>78</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="G17" s="4" t="s">
         <v>103</v>
       </c>
       <c r="I17" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:11">
       <c r="A18" t="s">
         <v>48</v>
       </c>
       <c r="B18" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="4" t="s">
         <v>110</v>
       </c>
       <c r="E18" t="s">
         <v>79</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="G18" s="4" t="s">
         <v>104</v>
       </c>
       <c r="I18" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:11">
       <c r="A19" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="4" t="s">
         <v>111</v>
       </c>
       <c r="I19" t="s">
         <v>96</v>
       </c>
-      <c r="J19" s="5" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10">
+      <c r="K19" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
       <c r="A20" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="4" t="s">
         <v>112</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:11">
       <c r="A21" t="s">
         <v>54</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="4" t="s">
         <v>113</v>
       </c>
       <c r="I21" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:11">
       <c r="A22" t="s">
         <v>55</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="4" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:11">
       <c r="A23" t="s">
         <v>56</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="4" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:11">
       <c r="A24" t="s">
         <v>57</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="4" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:11">
       <c r="A25" t="s">
         <v>58</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="4" t="s">
         <v>108</v>
       </c>
     </row>

</xml_diff>

<commit_message>
allocated pins to the rest of the features.
</commit_message>
<xml_diff>
--- a/electronics/mbed-motherboard/pin-allocation.xlsx
+++ b/electronics/mbed-motherboard/pin-allocation.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="153">
   <si>
     <t>Pin Name</t>
   </si>
@@ -115,9 +115,6 @@
     <t>axes steppers</t>
   </si>
   <si>
-    <t>step/dir/enable + protect</t>
-  </si>
-  <si>
     <t>P0.9</t>
   </si>
   <si>
@@ -463,17 +460,32 @@
     <t>test all footprints</t>
   </si>
   <si>
-    <t>assign pins</t>
-  </si>
-  <si>
-    <t>assign protect pins</t>
+    <t>x protect</t>
+  </si>
+  <si>
+    <t>y protect</t>
+  </si>
+  <si>
+    <t>z protect</t>
+  </si>
+  <si>
+    <t>a protect</t>
+  </si>
+  <si>
+    <t>b protect</t>
+  </si>
+  <si>
+    <t>BUZZER</t>
+  </si>
+  <si>
+    <t>SPINDLE RELAY</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -521,13 +533,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="16"/>
       <color theme="1"/>
@@ -651,24 +656,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="85">
@@ -1085,10 +1089,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1098,29 +1102,29 @@
     <col min="9" max="9" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="E2" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -1134,14 +1138,11 @@
         <f t="shared" ref="D3:D4" si="0">B3*C3</f>
         <v>20</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="F3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="E3" s="8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -1157,10 +1158,10 @@
         <v>5</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
         <v>28</v>
       </c>
@@ -1176,10 +1177,10 @@
         <v>10</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1194,10 +1195,10 @@
         <v>1</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -1212,10 +1213,10 @@
         <v>1</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
@@ -1230,10 +1231,10 @@
         <v>4</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="2" t="s">
         <v>19</v>
       </c>
@@ -1248,10 +1249,10 @@
         <v>1</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -1266,10 +1267,10 @@
         <v>1</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="2" t="s">
         <v>22</v>
       </c>
@@ -1284,10 +1285,10 @@
         <v>2</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="2" t="s">
         <v>23</v>
       </c>
@@ -1301,11 +1302,11 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E12" s="5" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="E12" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
@@ -1320,10 +1321,10 @@
         <v>3</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="2" t="s">
         <v>25</v>
       </c>
@@ -1338,10 +1339,10 @@
         <v>3</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" s="2" t="s">
         <v>26</v>
       </c>
@@ -1356,10 +1357,10 @@
         <v>1</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="3" t="s">
@@ -1393,37 +1394,32 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -1442,27 +1438,30 @@
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="11" max="11" width="14.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="20">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="E1" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="E1" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="I1" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="I1" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
@@ -1472,7 +1471,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>0</v>
@@ -1481,7 +1480,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>0</v>
@@ -1490,12 +1489,12 @@
         <v>1</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -1504,27 +1503,27 @@
         <v>3</v>
       </c>
       <c r="E3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" t="s">
         <v>59</v>
       </c>
-      <c r="F3" t="s">
-        <v>60</v>
-      </c>
       <c r="G3" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J3" t="s">
+        <v>124</v>
+      </c>
+      <c r="K3" s="4" t="s">
         <v>125</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -1533,24 +1532,24 @@
         <v>3</v>
       </c>
       <c r="E4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F4" t="s">
         <v>61</v>
       </c>
-      <c r="F4" t="s">
-        <v>62</v>
-      </c>
       <c r="G4" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
@@ -1559,142 +1558,151 @@
         <v>3</v>
       </c>
       <c r="E5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F5" t="s">
         <v>63</v>
       </c>
-      <c r="F5" t="s">
-        <v>64</v>
-      </c>
       <c r="G5" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F6" t="s">
         <v>65</v>
       </c>
-      <c r="F6" t="s">
-        <v>66</v>
-      </c>
       <c r="G6" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F7" t="s">
         <v>67</v>
       </c>
-      <c r="F7" t="s">
-        <v>68</v>
-      </c>
       <c r="G7" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I7" t="s">
-        <v>84</v>
+        <v>83</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I8" t="s">
-        <v>86</v>
+        <v>85</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B9" t="s">
         <v>2</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I9" t="s">
-        <v>87</v>
+        <v>86</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B10" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
@@ -1703,21 +1711,24 @@
         <v>22</v>
       </c>
       <c r="E11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I11" t="s">
-        <v>88</v>
+        <v>87</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
@@ -1726,210 +1737,219 @@
         <v>22</v>
       </c>
       <c r="E12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I12" t="s">
-        <v>89</v>
+        <v>88</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I14" t="s">
-        <v>91</v>
+        <v>90</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B15" t="s">
         <v>10</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I15" t="s">
-        <v>92</v>
+        <v>91</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B16" t="s">
         <v>10</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B17" t="s">
         <v>10</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:11">
       <c r="A18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B18" t="s">
         <v>10</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:11">
       <c r="A19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:11">
       <c r="A22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25" spans="1:11">
       <c r="A25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -1938,7 +1958,7 @@
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="I1:K1"/>
   </mergeCells>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
started routing power signals and shifted some parts around.
</commit_message>
<xml_diff>
--- a/electronics/mbed-motherboard/pin-allocation.xlsx
+++ b/electronics/mbed-motherboard/pin-allocation.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="154">
   <si>
     <t>Pin Name</t>
   </si>
@@ -479,6 +479,9 @@
   </si>
   <si>
     <t>SPINDLE RELAY</t>
+  </si>
+  <si>
+    <t>remove makerbot from botstep23 socket silk</t>
   </si>
 </sst>
 </file>
@@ -569,8 +572,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="85">
+  <cellStyleXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -668,14 +675,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="85">
+  <cellStyles count="89">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -718,6 +725,8 @@
     <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -760,6 +769,8 @@
     <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1089,10 +1100,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1138,7 +1149,7 @@
         <f t="shared" ref="D3:D4" si="0">B3*C3</f>
         <v>20</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="7" t="s">
         <v>123</v>
       </c>
     </row>
@@ -1420,6 +1431,11 @@
     <row r="25" spans="1:4">
       <c r="A25" t="s">
         <v>145</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -1447,21 +1463,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="20">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="E1" s="7" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="E1" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="I1" s="7" t="s">
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="I1" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">

</xml_diff>

<commit_message>
routed more of the board.  a couple pin swaps.
</commit_message>
<xml_diff>
--- a/electronics/mbed-motherboard/pin-allocation.xlsx
+++ b/electronics/mbed-motherboard/pin-allocation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1102,7 +1102,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
@@ -1453,8 +1453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1776,7 +1776,7 @@
         <v>10</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E13" t="s">
         <v>73</v>
@@ -1799,7 +1799,7 @@
         <v>10</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E14" t="s">
         <v>74</v>

</xml_diff>

<commit_message>
added holes, and dealt with more power supply routing stuff.  added power leds too.
</commit_message>
<xml_diff>
--- a/electronics/mbed-motherboard/pin-allocation.xlsx
+++ b/electronics/mbed-motherboard/pin-allocation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="153">
   <si>
     <t>Pin Name</t>
   </si>
@@ -445,12 +445,6 @@
     <t>more todo:</t>
   </si>
   <si>
-    <t>power leds</t>
-  </si>
-  <si>
-    <t>screw holes</t>
-  </si>
-  <si>
     <t>silkscreen</t>
   </si>
   <si>
@@ -482,6 +476,9 @@
   </si>
   <si>
     <t>remove makerbot from botstep23 socket silk</t>
+  </si>
+  <si>
+    <t>add net classes to high voltage lines (spindle, mosfets, etc)</t>
   </si>
 </sst>
 </file>
@@ -1100,10 +1097,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1425,17 +1422,12 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -1453,7 +1445,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView topLeftCell="A11" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -1635,7 +1627,7 @@
         <v>83</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1661,7 +1653,7 @@
         <v>85</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1687,7 +1679,7 @@
         <v>86</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1739,7 +1731,7 @@
         <v>87</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1765,7 +1757,7 @@
         <v>88</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1811,7 +1803,7 @@
         <v>90</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1834,7 +1826,7 @@
         <v>91</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="16" spans="1:11">

</xml_diff>

<commit_message>
cleaned up my library and rewired a bunch of stuff. ready for a rename now.
</commit_message>
<xml_diff>
--- a/electronics/mbed-motherboard/pin-allocation.xlsx
+++ b/electronics/mbed-motherboard/pin-allocation.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="152">
   <si>
     <t>Pin Name</t>
   </si>
@@ -473,9 +473,6 @@
   </si>
   <si>
     <t>SPINDLE RELAY</t>
-  </si>
-  <si>
-    <t>remove makerbot from botstep23 socket silk</t>
   </si>
   <si>
     <t>add net classes to high voltage lines (spindle, mosfets, etc)</t>
@@ -569,8 +566,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="89">
+  <cellStyleXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -679,7 +680,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="89">
+  <cellStyles count="93">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -724,6 +725,8 @@
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -768,6 +771,8 @@
     <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1097,10 +1102,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1407,27 +1412,22 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>